<commit_message>
completed clearance checking for url #1 and working on url#2
</commit_message>
<xml_diff>
--- a/db_check.xlsx
+++ b/db_check.xlsx
@@ -322,45 +322,60 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="26.5703125" customWidth="1" min="3" max="3"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t xml:space="preserve">First Name </t>
+          <t xml:space="preserve">Last Name </t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t xml:space="preserve">Last Name </t>
+          <t>First Name</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t xml:space="preserve">Clr check </t>
+          <t xml:space="preserve">Restults for URL1 </t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Bella</t>
+          <t>Moore</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Yang </t>
+          <t>Marie</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>No Results</t>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>headword</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Yes</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added and combined b_url check, a_url check, excel manip, and word manip
</commit_message>
<xml_diff>
--- a/db_check.xlsx
+++ b/db_check.xlsx
@@ -322,18 +322,18 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="22.140625" customWidth="1" min="1" max="1"/>
-    <col width="23.5703125" customWidth="1" min="2" max="2"/>
-    <col width="26.5703125" customWidth="1" min="3" max="3"/>
-    <col width="24.85546875" customWidth="1" min="4" max="4"/>
+    <col width="23.5703125" customWidth="1" min="2" max="6"/>
+    <col width="26.5703125" customWidth="1" min="7" max="7"/>
+    <col width="24.85546875" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -349,15 +349,35 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>Date_Created</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Date_Expired</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Institution</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">City, State </t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
           <t>URL1</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>URL2</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>URL3</t>
         </is>
@@ -374,13 +394,167 @@
           <t>Marie</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Yes</t>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Yes, individual appears on this list</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hello World </t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hello world </t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>No, individual is not listed</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Achiron</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Anat</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>No, individual is not listed</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Afsar</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Salman</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>No, individual is not listed</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Akgun</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Katia</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>No, individual is not listed</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Alroughani</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Raed</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>No, individual is not listed</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Bass</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Ann</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>No, individual is not listed</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Berkovich</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Regina</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>No, individual is not listed</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Broadley</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Simon</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>No, individual is not listed</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Celius</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Elisabeth</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>No, individual is not listed</t>
         </is>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added a sheet2 for rejected authors
</commit_message>
<xml_diff>
--- a/db_check.xlsx
+++ b/db_check.xlsx
@@ -3,10 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6900" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6900" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="sheet2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="sheet21" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="sheet22" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -15,7 +18,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <name val="Calibri"/>
@@ -45,8 +50,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -324,8 +330,8 @@
   </sheetPr>
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
@@ -394,9 +400,20 @@
           <t>Marie</t>
         </is>
       </c>
+      <c r="C2" s="1" t="n">
+        <v>43760.61611694683</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>44126.61611694683</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Yes, individual appears on this list</t>
+        </is>
+      </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Yes, individual appears on this list</t>
+          <t>No, individual is not listed</t>
         </is>
       </c>
     </row>
@@ -411,6 +428,17 @@
           <t xml:space="preserve">Hello world </t>
         </is>
       </c>
+      <c r="C3" s="1" t="n">
+        <v>43760.61614441942</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>44126.61614441942</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>No, individual is not listed</t>
+        </is>
+      </c>
       <c r="H3" t="inlineStr">
         <is>
           <t>No, individual is not listed</t>
@@ -428,6 +456,17 @@
           <t>Anat</t>
         </is>
       </c>
+      <c r="C4" s="1" t="n">
+        <v>43760.61617156792</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>44126.61617156792</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>No, individual is not listed</t>
+        </is>
+      </c>
       <c r="H4" t="inlineStr">
         <is>
           <t>No, individual is not listed</t>
@@ -445,6 +484,17 @@
           <t>Salman</t>
         </is>
       </c>
+      <c r="C5" s="1" t="n">
+        <v>43760.61619973052</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>44126.61619973052</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>No, individual is not listed</t>
+        </is>
+      </c>
       <c r="H5" t="inlineStr">
         <is>
           <t>No, individual is not listed</t>
@@ -462,6 +512,17 @@
           <t>Katia</t>
         </is>
       </c>
+      <c r="C6" s="1" t="n">
+        <v>43760.6162252288</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>44126.6162252288</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>No, individual is not listed</t>
+        </is>
+      </c>
       <c r="H6" t="inlineStr">
         <is>
           <t>No, individual is not listed</t>
@@ -479,6 +540,17 @@
           <t>Raed</t>
         </is>
       </c>
+      <c r="C7" s="1" t="n">
+        <v>43760.61624953821</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>44126.61624953821</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>No, individual is not listed</t>
+        </is>
+      </c>
       <c r="H7" t="inlineStr">
         <is>
           <t>No, individual is not listed</t>
@@ -496,6 +568,17 @@
           <t>Ann</t>
         </is>
       </c>
+      <c r="C8" s="1" t="n">
+        <v>43760.61627357056</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>44126.61627357056</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>No, individual is not listed</t>
+        </is>
+      </c>
       <c r="H8" t="inlineStr">
         <is>
           <t>No, individual is not listed</t>
@@ -513,6 +596,17 @@
           <t>Regina</t>
         </is>
       </c>
+      <c r="C9" s="1" t="n">
+        <v>43760.6162977645</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>44126.6162977645</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>No, individual is not listed</t>
+        </is>
+      </c>
       <c r="H9" t="inlineStr">
         <is>
           <t>No, individual is not listed</t>
@@ -530,6 +624,17 @@
           <t>Simon</t>
         </is>
       </c>
+      <c r="C10" s="1" t="n">
+        <v>43760.61632270875</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>44126.61632270875</v>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>No, individual is not listed</t>
+        </is>
+      </c>
       <c r="H10" t="inlineStr">
         <is>
           <t>No, individual is not listed</t>
@@ -545,6 +650,17 @@
       <c r="B11" t="inlineStr">
         <is>
           <t>Elisabeth</t>
+        </is>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>43760.61634633726</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>44126.61634633726</v>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>No, individual is not listed</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -557,4 +673,258 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">hello world </t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>hello world</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">hello world </t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">hello world </t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">hello world </t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">hello world </t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">hello world </t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">hello world </t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">hello world </t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">hello world </t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">hello world </t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">hello world </t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">hello world </t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">hello world </t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">hello world </t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">hello world </t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">hello world </t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Hiiii</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Hiiii</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Moore</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hello World </t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Achiron</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Afsar</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Akgun</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Alroughani</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Bass</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Berkovich</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Broadley</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Celius</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
committing updated files for dbBot, url2 and 3 were not needed anymore. Edited the word document generator.
</commit_message>
<xml_diff>
--- a/db_check.xlsx
+++ b/db_check.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6900" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6900" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -328,17 +328,17 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="22.140625" customWidth="1" min="1" max="1"/>
     <col width="23.5703125" customWidth="1" min="2" max="6"/>
-    <col width="26.5703125" customWidth="1" min="7" max="7"/>
+    <col width="34.140625" customWidth="1" min="7" max="7"/>
     <col width="24.85546875" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
@@ -380,12 +380,7 @@
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>URL2</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>URL3</t>
+          <t>Contributer</t>
         </is>
       </c>
     </row>
@@ -401,10 +396,20 @@
         </is>
       </c>
       <c r="C2" s="1" t="n">
-        <v>43760.61611694683</v>
+        <v>43762.61361264891</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>44126.61611694683</v>
+        <v>44128.61361264891</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -413,7 +418,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>No, individual is not listed</t>
+          <t>Bella</t>
         </is>
       </c>
     </row>
@@ -429,10 +434,20 @@
         </is>
       </c>
       <c r="C3" s="1" t="n">
-        <v>43760.61614441942</v>
+        <v>43762.61364490058</v>
       </c>
       <c r="D3" s="1" t="n">
-        <v>44126.61614441942</v>
+        <v>44128.61364490058</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -441,7 +456,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>No, individual is not listed</t>
+          <t>Bella</t>
         </is>
       </c>
     </row>
@@ -457,10 +472,20 @@
         </is>
       </c>
       <c r="C4" s="1" t="n">
-        <v>43760.61617156792</v>
+        <v>43762.61366567847</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>44126.61617156792</v>
+        <v>44128.61366567847</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -469,7 +494,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>No, individual is not listed</t>
+          <t>Bella</t>
         </is>
       </c>
     </row>
@@ -485,10 +510,20 @@
         </is>
       </c>
       <c r="C5" s="1" t="n">
-        <v>43760.61619973052</v>
+        <v>43762.61368709357</v>
       </c>
       <c r="D5" s="1" t="n">
-        <v>44126.61619973052</v>
+        <v>44128.61368709357</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -497,7 +532,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>No, individual is not listed</t>
+          <t>Bella</t>
         </is>
       </c>
     </row>
@@ -513,10 +548,20 @@
         </is>
       </c>
       <c r="C6" s="1" t="n">
-        <v>43760.6162252288</v>
+        <v>43762.61370829852</v>
       </c>
       <c r="D6" s="1" t="n">
-        <v>44126.6162252288</v>
+        <v>44128.61370829852</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -525,7 +570,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>No, individual is not listed</t>
+          <t>Bella</t>
         </is>
       </c>
     </row>
@@ -541,10 +586,20 @@
         </is>
       </c>
       <c r="C7" s="1" t="n">
-        <v>43760.61624953821</v>
+        <v>43762.61373041893</v>
       </c>
       <c r="D7" s="1" t="n">
-        <v>44126.61624953821</v>
+        <v>44128.61373041893</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -553,7 +608,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>No, individual is not listed</t>
+          <t>Bella</t>
         </is>
       </c>
     </row>
@@ -569,10 +624,20 @@
         </is>
       </c>
       <c r="C8" s="1" t="n">
-        <v>43760.61627357056</v>
+        <v>43762.61375293967</v>
       </c>
       <c r="D8" s="1" t="n">
-        <v>44126.61627357056</v>
+        <v>44128.61375293967</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -581,7 +646,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>No, individual is not listed</t>
+          <t>Bella</t>
         </is>
       </c>
     </row>
@@ -597,10 +662,20 @@
         </is>
       </c>
       <c r="C9" s="1" t="n">
-        <v>43760.6162977645</v>
+        <v>43762.6137754529</v>
       </c>
       <c r="D9" s="1" t="n">
-        <v>44126.6162977645</v>
+        <v>44128.6137754529</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -609,7 +684,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>No, individual is not listed</t>
+          <t>Bella</t>
         </is>
       </c>
     </row>
@@ -625,10 +700,20 @@
         </is>
       </c>
       <c r="C10" s="1" t="n">
-        <v>43760.61632270875</v>
+        <v>43762.61379878169</v>
       </c>
       <c r="D10" s="1" t="n">
-        <v>44126.61632270875</v>
+        <v>44128.61379878169</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -637,7 +722,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>No, individual is not listed</t>
+          <t>Bella</t>
         </is>
       </c>
     </row>
@@ -653,10 +738,20 @@
         </is>
       </c>
       <c r="C11" s="1" t="n">
-        <v>43760.61634633726</v>
+        <v>43762.61382257242</v>
       </c>
       <c r="D11" s="1" t="n">
-        <v>44126.61634633726</v>
+        <v>44128.61382257242</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -665,7 +760,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>No, individual is not listed</t>
+          <t>Bella</t>
         </is>
       </c>
     </row>
@@ -683,8 +778,8 @@
   </sheetPr>
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A1:A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
commiting edited files for the whole bot system
</commit_message>
<xml_diff>
--- a/db_check.xlsx
+++ b/db_check.xlsx
@@ -3,13 +3,11 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6900" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6900" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="sheet2" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="sheet21" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="sheet22" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -330,8 +328,8 @@
   </sheetPr>
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
@@ -396,10 +394,10 @@
         </is>
       </c>
       <c r="C2" s="1" t="n">
-        <v>43762.61361264891</v>
+        <v>43774.56153272498</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>44128.61361264891</v>
+        <v>44140.56153272498</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -434,10 +432,10 @@
         </is>
       </c>
       <c r="C3" s="1" t="n">
-        <v>43762.61364490058</v>
+        <v>43774.56155384894</v>
       </c>
       <c r="D3" s="1" t="n">
-        <v>44128.61364490058</v>
+        <v>44140.56155384894</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -472,10 +470,10 @@
         </is>
       </c>
       <c r="C4" s="1" t="n">
-        <v>43762.61366567847</v>
+        <v>43774.56157276814</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>44128.61366567847</v>
+        <v>44140.56157276814</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -510,10 +508,10 @@
         </is>
       </c>
       <c r="C5" s="1" t="n">
-        <v>43762.61368709357</v>
+        <v>43774.56159252999</v>
       </c>
       <c r="D5" s="1" t="n">
-        <v>44128.61368709357</v>
+        <v>44140.56159252999</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -548,10 +546,10 @@
         </is>
       </c>
       <c r="C6" s="1" t="n">
-        <v>43762.61370829852</v>
+        <v>43774.56161263816</v>
       </c>
       <c r="D6" s="1" t="n">
-        <v>44128.61370829852</v>
+        <v>44140.56161263816</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -586,10 +584,10 @@
         </is>
       </c>
       <c r="C7" s="1" t="n">
-        <v>43762.61373041893</v>
+        <v>43774.56163414304</v>
       </c>
       <c r="D7" s="1" t="n">
-        <v>44128.61373041893</v>
+        <v>44140.56163414304</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -624,10 +622,10 @@
         </is>
       </c>
       <c r="C8" s="1" t="n">
-        <v>43762.61375293967</v>
+        <v>43774.5616531315</v>
       </c>
       <c r="D8" s="1" t="n">
-        <v>44128.61375293967</v>
+        <v>44140.5616531315</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -662,10 +660,10 @@
         </is>
       </c>
       <c r="C9" s="1" t="n">
-        <v>43762.6137754529</v>
+        <v>43774.5616714393</v>
       </c>
       <c r="D9" s="1" t="n">
-        <v>44128.6137754529</v>
+        <v>44140.5616714393</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -700,10 +698,10 @@
         </is>
       </c>
       <c r="C10" s="1" t="n">
-        <v>43762.61379878169</v>
+        <v>43774.56169124693</v>
       </c>
       <c r="D10" s="1" t="n">
-        <v>44128.61379878169</v>
+        <v>44140.56169124693</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -738,10 +736,10 @@
         </is>
       </c>
       <c r="C11" s="1" t="n">
-        <v>43762.61382257242</v>
+        <v>43774.5617110323</v>
       </c>
       <c r="D11" s="1" t="n">
-        <v>44128.61382257242</v>
+        <v>44140.5617110323</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -776,250 +774,1539 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C27"/>
+  <dimension ref="A2:H53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A1:A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">hello world </t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>hello world</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">hello world </t>
-        </is>
-      </c>
-    </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t xml:space="preserve">hello world </t>
+          <t xml:space="preserve">Hello World </t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hello world </t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>2019-11-04 12:05:06.818975</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2020-11-04 12:05:06.818975</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>No, individual is not listed</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Bella</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t xml:space="preserve">hello world </t>
+          <t>Achiron</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Anat</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>2019-11-04 12:05:08.506166</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2020-11-04 12:05:08.506166</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>No, individual is not listed</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Bella</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t xml:space="preserve">hello world </t>
+          <t>Afsar</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Salman</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>2019-11-04 12:05:10.494772</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2020-11-04 12:05:10.494772</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>No, individual is not listed</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Bella</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t xml:space="preserve">hello world </t>
+          <t>Akgun</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Katia</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>2019-11-04 12:05:12.534219</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2020-11-04 12:05:12.534219</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>No, individual is not listed</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Bella</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t xml:space="preserve">hello world </t>
+          <t>Alroughani</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Raed</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2019-11-04 12:05:14.477018</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2020-11-04 12:05:14.477018</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>No, individual is not listed</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Bella</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t xml:space="preserve">hello world </t>
+          <t>Bass</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Ann</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>2019-11-04 12:05:16.475899</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2020-11-04 12:05:16.475899</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>No, individual is not listed</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Bella</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t xml:space="preserve">hello world </t>
+          <t>Berkovich</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Regina</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>2019-11-04 12:05:18.244056</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2020-11-04 12:05:18.244056</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>No, individual is not listed</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Bella</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t xml:space="preserve">hello world </t>
+          <t>Broadley</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Simon</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>2019-11-04 12:05:20.042771</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>2020-11-04 12:05:20.042771</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>No, individual is not listed</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Bella</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t xml:space="preserve">hello world </t>
+          <t>Celius</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Elisabeth</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>2019-11-04 12:05:21.846197</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>2020-11-04 12:05:21.846197</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>No, individual is not listed</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Bella</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t xml:space="preserve">hello world </t>
+          <t xml:space="preserve">Hello World </t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hello world </t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t xml:space="preserve">hello world </t>
+          <t>Achiron</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>2019-11-04 12:06:34.022912</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t xml:space="preserve">hello world </t>
+          <t>Afsar</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>2020-11-04 12:06:35.826677</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t xml:space="preserve">hello world </t>
+          <t>Akgun</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Temple University</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t xml:space="preserve">hello world </t>
+          <t>Alroughani</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Hiiii</t>
+          <t>Bass</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>No, individual is not listed</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Hiiii</t>
+          <t>Berkovich</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Bella</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Moore</t>
+          <t xml:space="preserve">Hello World </t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hello world </t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>2019-11-05 12:55:12.030209</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>2020-11-05 12:55:12.030209</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hello World </t>
+          <t>Achiron</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Anat</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>2019-11-05 12:55:14.024853</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>2020-11-05 12:55:14.024853</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Achiron</t>
+          <t>Afsar</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Salman</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>2019-11-05 12:55:15.581765</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>2020-11-05 12:55:15.581765</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Afsar</t>
+          <t>Akgun</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Katia</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>2019-11-05 12:55:17.290365</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>2020-11-05 12:55:17.290365</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Akgun</t>
+          <t>Alroughani</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Raed</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>2019-11-05 12:55:18.647715</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>2020-11-05 12:55:18.647715</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Alroughani</t>
+          <t>Bass</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Ann</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>2019-11-05 12:55:20.476802</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>2020-11-05 12:55:20.476802</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Bass</t>
+          <t>Berkovich</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Regina</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>2019-11-05 12:55:22.190199</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>2020-11-05 12:55:22.190199</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Berkovich</t>
+          <t>Broadley</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Simon</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>2019-11-04 12:06:44.218450</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>2020-11-04 12:06:44.218450</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Broadley</t>
+          <t>Celius</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Elisabeth</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>2019-11-04 12:06:45.938004</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>2020-11-04 12:06:45.938004</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
+          <t xml:space="preserve">Hello World </t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hello world </t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>2019-11-05 13:11:05.497320</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>2020-11-05 13:11:05.497320</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Achiron</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Anat</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>2019-11-05 13:11:06.961428</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>2020-11-05 13:11:06.961428</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Afsar</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Salman</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>2019-11-05 13:11:08.527280</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>2020-11-05 13:11:08.527280</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Akgun</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Katia</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>2019-11-05 13:11:09.967441</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>2020-11-05 13:11:09.967441</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Alroughani</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Raed</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>2019-11-05 13:11:11.640378</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>2020-11-05 13:11:11.640378</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Bass</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Ann</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>2019-11-05 13:11:13.086154</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>2020-11-05 13:11:13.086154</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Berkovich</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Regina</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>2019-11-05 13:11:15.229466</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>2020-11-05 13:11:15.229466</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Broadley</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Simon</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>2019-11-05 13:11:17.027275</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>2020-11-05 13:11:17.027275</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
           <t>Celius</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Elisabeth</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>2019-11-05 13:11:18.695119</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>2020-11-05 13:11:18.695119</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hello World </t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hello world </t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>2019-11-05 13:14:37.055319</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>2020-11-05 13:14:37.055319</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Achiron</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Anat</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>2019-11-05 13:14:38.903799</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>2020-11-05 13:14:38.903799</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Afsar</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Salman</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>2019-11-05 13:14:40.787779</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>2020-11-05 13:14:40.787779</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Akgun</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Katia</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>2019-11-05 13:14:42.304025</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>2020-11-05 13:14:42.304025</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Alroughani</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Raed</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>2019-11-05 13:14:44.012568</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>2020-11-05 13:14:44.012568</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Bass</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Ann</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>2019-11-05 13:14:45.300287</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>2020-11-05 13:14:45.300287</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Berkovich</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Regina</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>2019-11-05 13:14:46.863160</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>2020-11-05 13:14:46.863160</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Broadley</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Simon</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>2019-11-05 13:14:48.335196</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>2020-11-05 13:14:48.335196</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Celius</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Elisabeth</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>2019-11-05 13:14:49.866153</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>2020-11-05 13:14:49.866153</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hello World </t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hello world </t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>2019-11-05 13:25:18.891156</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>2020-11-05 13:25:18.891156</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Achiron</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Anat</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>2019-11-05 13:25:20.215593</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>2020-11-05 13:25:20.215593</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Afsar</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Salman</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>2019-11-05 13:25:21.510131</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>2020-11-05 13:25:21.510131</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Akgun</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Katia</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>2019-11-05 13:25:22.983140</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>2020-11-05 13:25:22.983140</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Alroughani</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Raed</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>2019-11-05 13:25:24.470173</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>2020-11-05 13:25:24.470173</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Bass</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Ann</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>2019-11-05 13:25:25.782624</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>2020-11-05 13:25:25.782624</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Berkovich</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Regina</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>2019-11-05 13:25:27.131009</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>2020-11-05 13:25:27.131009</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Broadley</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Simon</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>2019-11-05 13:25:31.276853</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>2020-11-05 13:25:31.276853</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Celius</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Elisabeth</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>2019-11-05 13:25:35.134057</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>2020-11-05 13:25:35.134057</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
         </is>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
cleaned up code commented functions
</commit_message>
<xml_diff>
--- a/db_check.xlsx
+++ b/db_check.xlsx
@@ -3,11 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6900" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6900" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="sheet2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Not Listed" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -328,11 +329,11 @@
   </sheetPr>
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="22.140625" customWidth="1" min="1" max="1"/>
     <col width="23.5703125" customWidth="1" min="2" max="6"/>
@@ -373,7 +374,7 @@
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>URL1</t>
+          <t xml:space="preserve">URL1 </t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
@@ -394,10 +395,10 @@
         </is>
       </c>
       <c r="C2" s="1" t="n">
-        <v>43774.56153272498</v>
+        <v>43781.59724796751</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>44140.56153272498</v>
+        <v>44147.59724796751</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -431,12 +432,8 @@
           <t xml:space="preserve">Hello world </t>
         </is>
       </c>
-      <c r="C3" s="1" t="n">
-        <v>43774.56155384894</v>
-      </c>
-      <c r="D3" s="1" t="n">
-        <v>44140.56155384894</v>
-      </c>
+      <c r="C3" s="1" t="n"/>
+      <c r="D3" s="1" t="n"/>
       <c r="E3" t="inlineStr">
         <is>
           <t>Temple University</t>
@@ -445,11 +442,6 @@
       <c r="F3" t="inlineStr">
         <is>
           <t xml:space="preserve">Phladelphia, PA </t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>No, individual is not listed</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -469,12 +461,8 @@
           <t>Anat</t>
         </is>
       </c>
-      <c r="C4" s="1" t="n">
-        <v>43774.56157276814</v>
-      </c>
-      <c r="D4" s="1" t="n">
-        <v>44140.56157276814</v>
-      </c>
+      <c r="C4" s="1" t="n"/>
+      <c r="D4" s="1" t="n"/>
       <c r="E4" t="inlineStr">
         <is>
           <t>Temple University</t>
@@ -483,11 +471,6 @@
       <c r="F4" t="inlineStr">
         <is>
           <t xml:space="preserve">Phladelphia, PA </t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>No, individual is not listed</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -507,12 +490,8 @@
           <t>Salman</t>
         </is>
       </c>
-      <c r="C5" s="1" t="n">
-        <v>43774.56159252999</v>
-      </c>
-      <c r="D5" s="1" t="n">
-        <v>44140.56159252999</v>
-      </c>
+      <c r="C5" s="1" t="n"/>
+      <c r="D5" s="1" t="n"/>
       <c r="E5" t="inlineStr">
         <is>
           <t>Temple University</t>
@@ -521,11 +500,6 @@
       <c r="F5" t="inlineStr">
         <is>
           <t xml:space="preserve">Phladelphia, PA </t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>No, individual is not listed</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -545,12 +519,8 @@
           <t>Katia</t>
         </is>
       </c>
-      <c r="C6" s="1" t="n">
-        <v>43774.56161263816</v>
-      </c>
-      <c r="D6" s="1" t="n">
-        <v>44140.56161263816</v>
-      </c>
+      <c r="C6" s="1" t="n"/>
+      <c r="D6" s="1" t="n"/>
       <c r="E6" t="inlineStr">
         <is>
           <t>Temple University</t>
@@ -559,11 +529,6 @@
       <c r="F6" t="inlineStr">
         <is>
           <t xml:space="preserve">Phladelphia, PA </t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>No, individual is not listed</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -583,12 +548,8 @@
           <t>Raed</t>
         </is>
       </c>
-      <c r="C7" s="1" t="n">
-        <v>43774.56163414304</v>
-      </c>
-      <c r="D7" s="1" t="n">
-        <v>44140.56163414304</v>
-      </c>
+      <c r="C7" s="1" t="n"/>
+      <c r="D7" s="1" t="n"/>
       <c r="E7" t="inlineStr">
         <is>
           <t>Temple University</t>
@@ -597,11 +558,6 @@
       <c r="F7" t="inlineStr">
         <is>
           <t xml:space="preserve">Phladelphia, PA </t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>No, individual is not listed</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -621,12 +577,8 @@
           <t>Ann</t>
         </is>
       </c>
-      <c r="C8" s="1" t="n">
-        <v>43774.5616531315</v>
-      </c>
-      <c r="D8" s="1" t="n">
-        <v>44140.5616531315</v>
-      </c>
+      <c r="C8" s="1" t="n"/>
+      <c r="D8" s="1" t="n"/>
       <c r="E8" t="inlineStr">
         <is>
           <t>Temple University</t>
@@ -635,11 +587,6 @@
       <c r="F8" t="inlineStr">
         <is>
           <t xml:space="preserve">Phladelphia, PA </t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>No, individual is not listed</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -659,12 +606,8 @@
           <t>Regina</t>
         </is>
       </c>
-      <c r="C9" s="1" t="n">
-        <v>43774.5616714393</v>
-      </c>
-      <c r="D9" s="1" t="n">
-        <v>44140.5616714393</v>
-      </c>
+      <c r="C9" s="1" t="n"/>
+      <c r="D9" s="1" t="n"/>
       <c r="E9" t="inlineStr">
         <is>
           <t>Temple University</t>
@@ -673,11 +616,6 @@
       <c r="F9" t="inlineStr">
         <is>
           <t xml:space="preserve">Phladelphia, PA </t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>No, individual is not listed</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -697,12 +635,8 @@
           <t>Simon</t>
         </is>
       </c>
-      <c r="C10" s="1" t="n">
-        <v>43774.56169124693</v>
-      </c>
-      <c r="D10" s="1" t="n">
-        <v>44140.56169124693</v>
-      </c>
+      <c r="C10" s="1" t="n"/>
+      <c r="D10" s="1" t="n"/>
       <c r="E10" t="inlineStr">
         <is>
           <t>Temple University</t>
@@ -711,11 +645,6 @@
       <c r="F10" t="inlineStr">
         <is>
           <t xml:space="preserve">Phladelphia, PA </t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>No, individual is not listed</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -735,12 +664,8 @@
           <t>Elisabeth</t>
         </is>
       </c>
-      <c r="C11" s="1" t="n">
-        <v>43774.5617110323</v>
-      </c>
-      <c r="D11" s="1" t="n">
-        <v>44140.5617110323</v>
-      </c>
+      <c r="C11" s="1" t="n"/>
+      <c r="D11" s="1" t="n"/>
       <c r="E11" t="inlineStr">
         <is>
           <t>Temple University</t>
@@ -749,11 +674,6 @@
       <c r="F11" t="inlineStr">
         <is>
           <t xml:space="preserve">Phladelphia, PA </t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>No, individual is not listed</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -774,354 +694,457 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:H53"/>
+  <dimension ref="A2:F126"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="D72" sqref="D72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="39.5703125" customWidth="1" min="4" max="4"/>
+  </cols>
   <sheetData>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hello World </t>
+          <t>Achiron</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hello world </t>
+          <t>Anat</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2019-11-04 12:05:06.818975</t>
+          <t>2019-11-05 12:55:14.024853</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2020-11-04 12:05:06.818975</t>
+          <t>2020-11-05 12:55:14.024853</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>No, individual is not listed</t>
+          <t>Temple University</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Bella</t>
+          <t xml:space="preserve">Phladelphia, PA </t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Achiron</t>
+          <t>Afsar</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Anat</t>
+          <t>Salman</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2019-11-04 12:05:08.506166</t>
+          <t>2019-11-05 12:55:15.581765</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2020-11-04 12:05:08.506166</t>
+          <t>2020-11-05 12:55:15.581765</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>No, individual is not listed</t>
+          <t>Temple University</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Bella</t>
+          <t xml:space="preserve">Phladelphia, PA </t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Afsar</t>
+          <t>Akgun</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Salman</t>
+          <t>Katia</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2019-11-04 12:05:10.494772</t>
+          <t>2019-11-05 12:55:17.290365</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2020-11-04 12:05:10.494772</t>
+          <t>2020-11-05 12:55:17.290365</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>No, individual is not listed</t>
+          <t>Temple University</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Bella</t>
+          <t xml:space="preserve">Phladelphia, PA </t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Akgun</t>
+          <t>Alroughani</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Katia</t>
+          <t>Raed</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2019-11-04 12:05:12.534219</t>
+          <t>2019-11-05 12:55:18.647715</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2020-11-04 12:05:12.534219</t>
+          <t>2020-11-05 12:55:18.647715</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>No, individual is not listed</t>
+          <t>Temple University</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Bella</t>
+          <t xml:space="preserve">Phladelphia, PA </t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Alroughani</t>
+          <t>Bass</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Raed</t>
+          <t>Ann</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2019-11-04 12:05:14.477018</t>
+          <t>2019-11-05 12:55:20.476802</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2020-11-04 12:05:14.477018</t>
+          <t>2020-11-05 12:55:20.476802</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>No, individual is not listed</t>
+          <t>Temple University</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Bella</t>
+          <t xml:space="preserve">Phladelphia, PA </t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Bass</t>
+          <t>Berkovich</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Ann</t>
+          <t>Regina</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2019-11-04 12:05:16.475899</t>
+          <t>2019-11-05 12:55:22.190199</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2020-11-04 12:05:16.475899</t>
+          <t>2020-11-05 12:55:22.190199</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>No, individual is not listed</t>
+          <t>Temple University</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Bella</t>
+          <t xml:space="preserve">Phladelphia, PA </t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Berkovich</t>
+          <t>Broadley</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Regina</t>
+          <t>Simon</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2019-11-04 12:05:18.244056</t>
+          <t>2019-11-04 12:06:44.218450</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2020-11-04 12:05:18.244056</t>
+          <t>2020-11-04 12:06:44.218450</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>No, individual is not listed</t>
+          <t>Temple University</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Bella</t>
+          <t xml:space="preserve">Phladelphia, PA </t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Broadley</t>
+          <t>Celius</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Simon</t>
+          <t>Elisabeth</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2019-11-04 12:05:20.042771</t>
+          <t>2019-11-04 12:06:45.938004</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2020-11-04 12:05:20.042771</t>
+          <t>2020-11-04 12:06:45.938004</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>No, individual is not listed</t>
+          <t>Temple University</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Bella</t>
+          <t xml:space="preserve">Phladelphia, PA </t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Celius</t>
+          <t xml:space="preserve">Hello World </t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Elisabeth</t>
+          <t xml:space="preserve">Hello world </t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2019-11-04 12:05:21.846197</t>
+          <t>2019-11-05 13:11:05.497320</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2020-11-04 12:05:21.846197</t>
+          <t>2020-11-05 13:11:05.497320</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>No, individual is not listed</t>
+          <t>Temple University</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Bella</t>
+          <t xml:space="preserve">Phladelphia, PA </t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hello World </t>
+          <t>Achiron</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hello world </t>
+          <t>Anat</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>2019-11-05 13:11:06.961428</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>2020-11-05 13:11:06.961428</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Achiron</t>
+          <t>Afsar</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Salman</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2019-11-04 12:06:34.022912</t>
+          <t>2019-11-05 13:11:08.527280</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>2020-11-05 13:11:08.527280</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Afsar</t>
+          <t>Akgun</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Katia</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>2019-11-05 13:11:09.967441</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2020-11-04 12:06:35.826677</t>
+          <t>2020-11-05 13:11:09.967441</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Akgun</t>
+          <t>Alroughani</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Raed</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>2019-11-05 13:11:11.640378</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>2020-11-05 13:11:11.640378</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
           <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Alroughani</t>
+          <t>Bass</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Ann</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>2019-11-05 13:11:13.086154</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>2020-11-05 13:11:13.086154</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Temple University</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1133,46 +1156,86 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Bass</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>No, individual is not listed</t>
+          <t>Berkovich</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Regina</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>2019-11-05 13:11:15.229466</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>2020-11-05 13:11:15.229466</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Berkovich</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>Bella</t>
+          <t>Broadley</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Simon</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>2019-11-05 13:11:17.027275</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>2020-11-05 13:11:17.027275</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hello World </t>
+          <t>Celius</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hello world </t>
+          <t>Elisabeth</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>2019-11-05 12:55:12.030209</t>
+          <t>2019-11-05 13:11:18.695119</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2020-11-05 12:55:12.030209</t>
+          <t>2020-11-05 13:11:18.695119</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1189,22 +1252,22 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Achiron</t>
+          <t xml:space="preserve">Hello World </t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Anat</t>
+          <t xml:space="preserve">Hello world </t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>2019-11-05 12:55:14.024853</t>
+          <t>2019-11-05 13:14:37.055319</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>2020-11-05 12:55:14.024853</t>
+          <t>2020-11-05 13:14:37.055319</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1221,22 +1284,22 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Afsar</t>
+          <t>Achiron</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Salman</t>
+          <t>Anat</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>2019-11-05 12:55:15.581765</t>
+          <t>2019-11-05 13:14:38.903799</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2020-11-05 12:55:15.581765</t>
+          <t>2020-11-05 13:14:38.903799</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1253,22 +1316,22 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Akgun</t>
+          <t>Afsar</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Katia</t>
+          <t>Salman</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>2019-11-05 12:55:17.290365</t>
+          <t>2019-11-05 13:14:40.787779</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>2020-11-05 12:55:17.290365</t>
+          <t>2020-11-05 13:14:40.787779</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1285,22 +1348,22 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Alroughani</t>
+          <t>Akgun</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Raed</t>
+          <t>Katia</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>2019-11-05 12:55:18.647715</t>
+          <t>2019-11-05 13:14:42.304025</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>2020-11-05 12:55:18.647715</t>
+          <t>2020-11-05 13:14:42.304025</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1317,22 +1380,22 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Bass</t>
+          <t>Alroughani</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Ann</t>
+          <t>Raed</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>2019-11-05 12:55:20.476802</t>
+          <t>2019-11-05 13:14:44.012568</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>2020-11-05 12:55:20.476802</t>
+          <t>2020-11-05 13:14:44.012568</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1349,22 +1412,22 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Berkovich</t>
+          <t>Bass</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Regina</t>
+          <t>Ann</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>2019-11-05 12:55:22.190199</t>
+          <t>2019-11-05 13:14:45.300287</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>2020-11-05 12:55:22.190199</t>
+          <t>2020-11-05 13:14:45.300287</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1381,22 +1444,22 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Broadley</t>
+          <t>Berkovich</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Simon</t>
+          <t>Regina</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>2019-11-04 12:06:44.218450</t>
+          <t>2019-11-05 13:14:46.863160</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>2020-11-04 12:06:44.218450</t>
+          <t>2020-11-05 13:14:46.863160</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1413,22 +1476,22 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Celius</t>
+          <t>Broadley</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Elisabeth</t>
+          <t>Simon</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>2019-11-04 12:06:45.938004</t>
+          <t>2019-11-05 13:14:48.335196</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>2020-11-04 12:06:45.938004</t>
+          <t>2020-11-05 13:14:48.335196</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1445,22 +1508,22 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hello World </t>
+          <t>Celius</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hello world </t>
+          <t>Elisabeth</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>2019-11-05 13:11:05.497320</t>
+          <t>2019-11-05 13:14:49.866153</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>2020-11-05 13:11:05.497320</t>
+          <t>2020-11-05 13:14:49.866153</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1477,22 +1540,22 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Achiron</t>
+          <t xml:space="preserve">Hello World </t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Anat</t>
+          <t xml:space="preserve">Hello world </t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>2019-11-05 13:11:06.961428</t>
+          <t>2019-11-05 13:25:18.891156</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>2020-11-05 13:11:06.961428</t>
+          <t>2020-11-05 13:25:18.891156</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -1509,22 +1572,22 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Afsar</t>
+          <t>Achiron</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Salman</t>
+          <t>Anat</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>2019-11-05 13:11:08.527280</t>
+          <t>2019-11-05 13:25:20.215593</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>2020-11-05 13:11:08.527280</t>
+          <t>2020-11-05 13:25:20.215593</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -1541,22 +1604,22 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Akgun</t>
+          <t>Afsar</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Katia</t>
+          <t>Salman</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>2019-11-05 13:11:09.967441</t>
+          <t>2019-11-05 13:25:21.510131</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>2020-11-05 13:11:09.967441</t>
+          <t>2020-11-05 13:25:21.510131</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -1573,22 +1636,22 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Alroughani</t>
+          <t>Akgun</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Raed</t>
+          <t>Katia</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>2019-11-05 13:11:11.640378</t>
+          <t>2019-11-05 13:25:22.983140</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>2020-11-05 13:11:11.640378</t>
+          <t>2020-11-05 13:25:22.983140</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -1605,22 +1668,22 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Bass</t>
+          <t>Alroughani</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Ann</t>
+          <t>Raed</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>2019-11-05 13:11:13.086154</t>
+          <t>2019-11-05 13:25:24.470173</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>2020-11-05 13:11:13.086154</t>
+          <t>2020-11-05 13:25:24.470173</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -1637,22 +1700,22 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Berkovich</t>
+          <t>Bass</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Regina</t>
+          <t>Ann</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>2019-11-05 13:11:15.229466</t>
+          <t>2019-11-05 13:25:25.782624</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>2020-11-05 13:11:15.229466</t>
+          <t>2020-11-05 13:25:25.782624</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -1669,22 +1732,22 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Broadley</t>
+          <t>Berkovich</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Simon</t>
+          <t>Regina</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>2019-11-05 13:11:17.027275</t>
+          <t>2019-11-05 13:25:27.131009</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>2020-11-05 13:11:17.027275</t>
+          <t>2020-11-05 13:25:27.131009</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -1701,22 +1764,22 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Celius</t>
+          <t>Broadley</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Elisabeth</t>
+          <t>Simon</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>2019-11-05 13:11:18.695119</t>
+          <t>2019-11-05 13:25:31.276853</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>2020-11-05 13:11:18.695119</t>
+          <t>2020-11-05 13:25:31.276853</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -1733,22 +1796,22 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hello World </t>
+          <t>Celius</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hello world </t>
+          <t>Elisabeth</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>2019-11-05 13:14:37.055319</t>
+          <t>2019-11-05 13:25:35.134057</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>2020-11-05 13:14:37.055319</t>
+          <t>2020-11-05 13:25:35.134057</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -1765,22 +1828,22 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Achiron</t>
+          <t xml:space="preserve">Hello World </t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Anat</t>
+          <t xml:space="preserve">Hello world </t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>2019-11-05 13:14:38.903799</t>
+          <t>2019-11-05 13:28:38.252548</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>2020-11-05 13:14:38.903799</t>
+          <t>2020-11-05 13:28:38.252548</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -1797,22 +1860,22 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Afsar</t>
+          <t>Achiron</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Salman</t>
+          <t>Anat</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>2019-11-05 13:14:40.787779</t>
+          <t>2019-11-05 13:28:39.887168</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>2020-11-05 13:14:40.787779</t>
+          <t>2020-11-05 13:28:39.887168</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -1829,22 +1892,22 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Akgun</t>
+          <t>Afsar</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Katia</t>
+          <t>Salman</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>2019-11-05 13:14:42.304025</t>
+          <t>2019-11-05 13:28:41.594591</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>2020-11-05 13:14:42.304025</t>
+          <t>2020-11-05 13:28:41.594591</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -1861,22 +1924,22 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Alroughani</t>
+          <t>Akgun</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Raed</t>
+          <t>Katia</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>2019-11-05 13:14:44.012568</t>
+          <t>2019-11-05 13:28:43.331937</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>2020-11-05 13:14:44.012568</t>
+          <t>2020-11-05 13:28:43.331937</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
@@ -1893,22 +1956,22 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Bass</t>
+          <t>Alroughani</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Ann</t>
+          <t>Raed</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>2019-11-05 13:14:45.300287</t>
+          <t>2019-11-05 13:28:45.189959</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>2020-11-05 13:14:45.300287</t>
+          <t>2020-11-05 13:28:45.189959</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
@@ -1925,22 +1988,22 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Berkovich</t>
+          <t>Bass</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Regina</t>
+          <t>Ann</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>2019-11-05 13:14:46.863160</t>
+          <t>2019-11-05 13:28:46.830562</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>2020-11-05 13:14:46.863160</t>
+          <t>2020-11-05 13:28:46.830562</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
@@ -1957,22 +2020,22 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Broadley</t>
+          <t>Berkovich</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Simon</t>
+          <t>Regina</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>2019-11-05 13:14:48.335196</t>
+          <t>2019-11-05 13:28:48.412356</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>2020-11-05 13:14:48.335196</t>
+          <t>2020-11-05 13:28:48.412356</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
@@ -1989,22 +2052,22 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Celius</t>
+          <t>Broadley</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Elisabeth</t>
+          <t>Simon</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>2019-11-05 13:14:49.866153</t>
+          <t>2019-11-05 13:28:50.123734</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>2020-11-05 13:14:49.866153</t>
+          <t>2020-11-05 13:28:50.123734</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
@@ -2021,22 +2084,22 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hello World </t>
+          <t>Celius</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hello world </t>
+          <t>Elisabeth</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>2019-11-05 13:25:18.891156</t>
+          <t>2019-11-05 13:28:51.833191</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>2020-11-05 13:25:18.891156</t>
+          <t>2020-11-05 13:28:51.833191</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
@@ -2053,22 +2116,22 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Achiron</t>
+          <t xml:space="preserve">Hello World </t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Anat</t>
+          <t xml:space="preserve">Hello world </t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>2019-11-05 13:25:20.215593</t>
+          <t>2019-11-11 09:06:32.168726</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>2020-11-05 13:25:20.215593</t>
+          <t>2020-11-11 09:06:32.168726</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
@@ -2085,22 +2148,22 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Afsar</t>
+          <t>Achiron</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Salman</t>
+          <t>Anat</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>2019-11-05 13:25:21.510131</t>
+          <t>2019-11-11 09:06:33.625836</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>2020-11-05 13:25:21.510131</t>
+          <t>2020-11-11 09:06:33.625836</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -2117,22 +2180,22 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Akgun</t>
+          <t xml:space="preserve">Hello World </t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Katia</t>
+          <t xml:space="preserve">Hello world </t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>2019-11-05 13:25:22.983140</t>
+          <t>2019-11-11 09:09:22.120877</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>2020-11-05 13:25:22.983140</t>
+          <t>2020-11-11 09:09:22.120877</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
@@ -2149,22 +2212,22 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Alroughani</t>
+          <t xml:space="preserve">Hello World </t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Raed</t>
+          <t xml:space="preserve">Hello world </t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>2019-11-05 13:25:24.470173</t>
+          <t>2019-11-11 09:11:23.032247</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>2020-11-05 13:25:24.470173</t>
+          <t>2020-11-11 09:11:23.032247</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
@@ -2181,22 +2244,22 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Bass</t>
+          <t>Achiron</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Ann</t>
+          <t>Anat</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>2019-11-05 13:25:25.782624</t>
+          <t>2019-11-11 09:09:23.825551</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>2020-11-05 13:25:25.782624</t>
+          <t>2020-11-11 09:09:23.825551</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
@@ -2213,22 +2276,22 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Berkovich</t>
+          <t>Afsar</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Regina</t>
+          <t>Salman</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>2019-11-05 13:25:27.131009</t>
+          <t>2019-11-11 09:06:35.037068</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>2020-11-05 13:25:27.131009</t>
+          <t>2020-11-11 09:06:35.037068</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
@@ -2245,22 +2308,22 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Broadley</t>
+          <t>Akgun</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Simon</t>
+          <t>Katia</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>2019-11-05 13:25:31.276853</t>
+          <t>2019-11-11 09:06:36.422365</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>2020-11-05 13:25:31.276853</t>
+          <t>2020-11-11 09:06:36.422365</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
@@ -2277,30 +2340,2366 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
+          <t>Alroughani</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Raed</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>2019-11-11 09:06:37.791707</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>2020-11-11 09:06:37.791707</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Bass</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Ann</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>2019-11-11 09:06:39.207924</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>2020-11-11 09:06:39.207924</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Berkovich</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Regina</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>2019-11-11 09:06:40.652068</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>2020-11-11 09:06:40.652068</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Broadley</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Simon</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>2019-11-11 09:06:42.300665</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>2020-11-11 09:06:42.300665</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
           <t>Celius</t>
         </is>
       </c>
-      <c r="B53" t="inlineStr">
+      <c r="B57" t="inlineStr">
         <is>
           <t>Elisabeth</t>
         </is>
       </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>2019-11-05 13:25:35.134057</t>
-        </is>
-      </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>2020-11-05 13:25:35.134057</t>
-        </is>
-      </c>
-      <c r="E53" t="inlineStr">
-        <is>
-          <t>Temple University</t>
-        </is>
-      </c>
-      <c r="F53" t="inlineStr">
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>2019-11-11 09:06:43.947304</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>2020-11-11 09:06:43.947304</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hello World </t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hello world </t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>2019-11-11 09:11:49.867126</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>2020-11-11 09:11:49.867126</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Achiron</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Anat</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>2019-11-11 09:11:52.680522</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>2020-11-11 09:11:52.680522</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Afsar</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Salman</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>2019-11-11 09:11:55.457838</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>2020-11-11 09:11:55.457838</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hello World </t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hello world </t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>2019-11-11 09:28:12.997485</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>2020-11-11 09:28:12.997485</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Achiron</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Anat</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>2019-11-11 09:28:15.382238</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>2020-11-11 09:28:15.382238</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Afsar</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Salman</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>2019-11-11 09:28:17.900649</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>2020-11-11 09:28:17.900649</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hello World </t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hello world </t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>2019-11-11 09:28:44.180225</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>2020-11-11 09:28:44.180225</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Achiron</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Anat</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>2019-11-11 09:28:46.804020</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>2020-11-11 09:28:46.804020</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Afsar</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Salman</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>2019-11-11 09:28:49.643957</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>2020-11-11 09:28:49.643957</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Akgun</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Katia</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>2019-11-11 09:11:58.165184</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>2020-11-11 09:11:58.165184</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Alroughani</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Raed</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>2019-11-11 09:12:00.937684</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>2020-11-11 09:12:00.937684</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Bass</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Ann</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>2019-11-11 09:12:03.583732</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>2020-11-11 09:12:03.583732</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Berkovich</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Regina</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>2019-11-11 09:12:06.161836</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>2020-11-11 09:12:06.161836</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Broadley</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Simon</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>2019-11-11 09:12:09.015785</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>2020-11-11 09:12:09.015785</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Celius</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Elisabeth</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>2019-11-11 09:12:11.946215</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>2020-11-11 09:12:11.946215</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hello World </t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hello world </t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Achiron</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Anat</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Afsar</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Salman</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Akgun</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Katia</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Alroughani</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Raed</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Bass</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Ann</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Berkovich</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Regina</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Broadley</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Simon</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>Celius</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>Elisabeth</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hello World </t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hello world </t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>2019-11-11 09:42:58.436172</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>2020-11-11 09:42:58.436172</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>Achiron</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>Anat</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>2019-11-11 09:43:01.206796</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>2020-11-11 09:43:01.206796</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>Afsar</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>Salman</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>2019-11-11 09:43:03.969436</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>2020-11-11 09:43:03.969436</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>Akgun</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>Katia</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>2019-11-11 09:43:06.717129</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>2020-11-11 09:43:06.717129</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>Alroughani</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>Raed</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>2019-11-11 09:43:09.550814</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>2020-11-11 09:43:09.550814</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>Bass</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Ann</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>2019-11-11 09:43:12.288233</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>2020-11-11 09:43:12.288233</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>Berkovich</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>Regina</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>2019-11-11 09:43:14.979125</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>2020-11-11 09:43:14.979125</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>Broadley</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>Simon</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>2019-11-11 09:43:17.871743</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>2020-11-11 09:43:17.871743</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>Celius</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>Elisabeth</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>2019-11-11 09:43:20.646944</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>2020-11-11 09:43:20.646944</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hello World </t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hello world </t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>Achiron</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>Anat</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>Afsar</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>Salman</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>Akgun</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>Katia</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>Alroughani</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>Raed</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>Bass</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>Ann</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>Berkovich</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>Regina</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>Broadley</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>Simon</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>Celius</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>Elisabeth</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hello World </t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hello world </t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>2019-11-11 10:25:08.745239</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>2020-11-11 10:25:08.745239</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>Achiron</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>Anat</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>2019-11-11 10:25:11.780700</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>2020-11-11 10:25:11.780700</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>Afsar</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>Salman</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>2019-11-11 10:25:14.778479</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>2020-11-11 10:25:14.778479</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>Akgun</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>Katia</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>2019-11-11 10:25:17.703044</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>2020-11-11 10:25:17.703044</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>Alroughani</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>Raed</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>2019-11-11 10:25:20.855321</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>2020-11-11 10:25:20.855321</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>Bass</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>Ann</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>2019-11-11 10:25:23.750554</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>2020-11-11 10:25:23.750554</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>Berkovich</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>Regina</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>2019-11-11 10:25:26.704081</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>2020-11-11 10:25:26.704081</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>Broadley</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>Simon</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>2019-11-11 10:25:29.791044</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>2020-11-11 10:25:29.791044</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>Celius</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>Elisabeth</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>2019-11-11 10:25:33.253383</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>2020-11-11 10:25:33.253383</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hello World </t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hello world </t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>2019-11-11 12:20:31.352014</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>2020-11-11 12:20:31.352014</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>Achiron</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>Anat</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>2019-11-11 12:20:33.061430</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>2020-11-11 12:20:33.061430</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>Afsar</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>Salman</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>2019-11-11 12:20:34.725965</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>2020-11-11 12:20:34.725965</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>Akgun</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>Katia</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>2019-11-11 12:20:36.777465</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>2020-11-11 12:20:36.777465</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>Alroughani</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>Raed</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>2019-11-11 12:20:38.675676</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>2020-11-11 12:20:38.675676</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>Bass</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>Ann</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>2019-11-11 12:20:40.270438</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>2020-11-11 12:20:40.270438</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>Berkovich</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>Regina</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>2019-11-11 12:20:42.009736</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>2020-11-11 12:20:42.009736</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>Broadley</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>Simon</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>2019-11-11 12:20:43.679259</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>2020-11-11 12:20:43.679259</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>Celius</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>Elisabeth</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>2019-11-11 12:20:45.513375</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>2020-11-11 12:20:45.513375</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hello World </t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hello world </t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>2019-11-11 12:21:21.654391</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>2020-11-11 12:21:21.654391</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F118" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>Achiron</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>Anat</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>2019-11-11 12:21:23.361862</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>2020-11-11 12:21:23.361862</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>Afsar</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>Salman</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>2019-11-11 12:21:24.987620</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>2020-11-11 12:21:24.987620</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>Akgun</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>Katia</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>2019-11-11 12:21:26.516523</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>2020-11-11 12:21:26.516523</t>
+        </is>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>Alroughani</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>Raed</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>2019-11-11 12:21:28.165265</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>2020-11-11 12:21:28.165265</t>
+        </is>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>Bass</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>Ann</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>2019-11-11 12:21:29.913201</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>2020-11-11 12:21:29.913201</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>Berkovich</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>Regina</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>2019-11-11 12:21:31.741498</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>2020-11-11 12:21:31.741498</t>
+        </is>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>Broadley</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>Simon</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>2019-11-11 12:21:33.495324</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>2020-11-11 12:21:33.495324</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F125" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>Celius</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>Elisabeth</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>2019-11-11 12:21:35.488207</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>2020-11-11 12:21:35.488207</t>
+        </is>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F126" t="inlineStr">
         <is>
           <t xml:space="preserve">Phladelphia, PA </t>
         </is>
@@ -2309,4 +4708,22 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added more file structure and cleaned some code and logic
</commit_message>
<xml_diff>
--- a/db_check.xlsx
+++ b/db_check.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6900" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6900" tabRatio="351" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -330,10 +330,10 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="22.140625" customWidth="1" min="1" max="1"/>
     <col width="23.5703125" customWidth="1" min="2" max="6"/>
@@ -395,10 +395,10 @@
         </is>
       </c>
       <c r="C2" s="1" t="n">
-        <v>43781.59724796751</v>
+        <v>43788.43747271357</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>44147.59724796751</v>
+        <v>44154.43747271357</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -432,8 +432,12 @@
           <t xml:space="preserve">Hello world </t>
         </is>
       </c>
-      <c r="C3" s="1" t="n"/>
-      <c r="D3" s="1" t="n"/>
+      <c r="C3" s="1" t="n">
+        <v>43788.43749121563</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>44154.43749121563</v>
+      </c>
       <c r="E3" t="inlineStr">
         <is>
           <t>Temple University</t>
@@ -442,6 +446,11 @@
       <c r="F3" t="inlineStr">
         <is>
           <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>No, individual is not listed</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -461,8 +470,12 @@
           <t>Anat</t>
         </is>
       </c>
-      <c r="C4" s="1" t="n"/>
-      <c r="D4" s="1" t="n"/>
+      <c r="C4" s="1" t="n">
+        <v>43788.4375108183</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>44154.4375108183</v>
+      </c>
       <c r="E4" t="inlineStr">
         <is>
           <t>Temple University</t>
@@ -471,6 +484,11 @@
       <c r="F4" t="inlineStr">
         <is>
           <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>No, individual is not listed</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -490,8 +508,12 @@
           <t>Salman</t>
         </is>
       </c>
-      <c r="C5" s="1" t="n"/>
-      <c r="D5" s="1" t="n"/>
+      <c r="C5" s="1" t="n">
+        <v>43788.43753119933</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>44154.43753119933</v>
+      </c>
       <c r="E5" t="inlineStr">
         <is>
           <t>Temple University</t>
@@ -500,6 +522,11 @@
       <c r="F5" t="inlineStr">
         <is>
           <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>No, individual is not listed</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -519,8 +546,12 @@
           <t>Katia</t>
         </is>
       </c>
-      <c r="C6" s="1" t="n"/>
-      <c r="D6" s="1" t="n"/>
+      <c r="C6" s="1" t="n">
+        <v>43788.43754984346</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>44154.43754984346</v>
+      </c>
       <c r="E6" t="inlineStr">
         <is>
           <t>Temple University</t>
@@ -529,6 +560,11 @@
       <c r="F6" t="inlineStr">
         <is>
           <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>No, individual is not listed</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -548,8 +584,12 @@
           <t>Raed</t>
         </is>
       </c>
-      <c r="C7" s="1" t="n"/>
-      <c r="D7" s="1" t="n"/>
+      <c r="C7" s="1" t="n">
+        <v>43788.43756985311</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>44154.43756985311</v>
+      </c>
       <c r="E7" t="inlineStr">
         <is>
           <t>Temple University</t>
@@ -558,6 +598,11 @@
       <c r="F7" t="inlineStr">
         <is>
           <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>No, individual is not listed</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -577,8 +622,12 @@
           <t>Ann</t>
         </is>
       </c>
-      <c r="C8" s="1" t="n"/>
-      <c r="D8" s="1" t="n"/>
+      <c r="C8" s="1" t="n">
+        <v>43788.43759630928</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>44154.43759630928</v>
+      </c>
       <c r="E8" t="inlineStr">
         <is>
           <t>Temple University</t>
@@ -587,6 +636,11 @@
       <c r="F8" t="inlineStr">
         <is>
           <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>No, individual is not listed</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -606,8 +660,12 @@
           <t>Regina</t>
         </is>
       </c>
-      <c r="C9" s="1" t="n"/>
-      <c r="D9" s="1" t="n"/>
+      <c r="C9" s="1" t="n">
+        <v>43788.43761429244</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>44154.43761429244</v>
+      </c>
       <c r="E9" t="inlineStr">
         <is>
           <t>Temple University</t>
@@ -616,6 +674,11 @@
       <c r="F9" t="inlineStr">
         <is>
           <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>No, individual is not listed</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -635,8 +698,12 @@
           <t>Simon</t>
         </is>
       </c>
-      <c r="C10" s="1" t="n"/>
-      <c r="D10" s="1" t="n"/>
+      <c r="C10" s="1" t="n">
+        <v>43788.43763458207</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>44154.43763458207</v>
+      </c>
       <c r="E10" t="inlineStr">
         <is>
           <t>Temple University</t>
@@ -645,6 +712,11 @@
       <c r="F10" t="inlineStr">
         <is>
           <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>No, individual is not listed</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -664,8 +736,12 @@
           <t>Elisabeth</t>
         </is>
       </c>
-      <c r="C11" s="1" t="n"/>
-      <c r="D11" s="1" t="n"/>
+      <c r="C11" s="1" t="n">
+        <v>43788.43765205468</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>44154.43765205468</v>
+      </c>
       <c r="E11" t="inlineStr">
         <is>
           <t>Temple University</t>
@@ -674,6 +750,11 @@
       <c r="F11" t="inlineStr">
         <is>
           <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>No, individual is not listed</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -700,7 +781,7 @@
       <selection activeCell="D72" sqref="D72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="39.5703125" customWidth="1" min="4" max="4"/>
   </cols>
@@ -4716,14 +4797,591 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A2:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hello World </t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hello world </t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>2019-11-14 15:06:43.151148</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2020-11-14 15:06:43.151148</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Achiron</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Anat</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>2019-11-14 15:06:46.292269</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2020-11-14 15:06:46.292269</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Afsar</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Salman</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>2019-11-14 15:06:50.515504</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2020-11-14 15:06:50.515504</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Akgun</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Katia</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>2019-11-14 15:06:53.411093</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2020-11-14 15:06:53.411093</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Alroughani</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Raed</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2019-11-14 15:06:56.647043</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2020-11-14 15:06:56.647043</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Bass</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Ann</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>2019-11-14 15:06:59.691783</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2020-11-14 15:06:59.691783</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Berkovich</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Regina</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>2019-11-14 15:07:02.691349</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2020-11-14 15:07:02.691349</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Broadley</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Simon</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>2019-11-14 15:07:05.790248</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>2020-11-14 15:07:05.790248</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Celius</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Elisabeth</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>2019-11-14 15:07:08.776399</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>2020-11-14 15:07:08.776399</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hello World </t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hello world </t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>2019-11-19 10:29:59.241031</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>2020-11-19 10:29:59.241031</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Achiron</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Anat</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>2019-11-19 10:30:00.934701</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>2020-11-19 10:30:00.934701</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Afsar</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Salman</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>2019-11-19 10:30:02.695622</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>2020-11-19 10:30:02.695622</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Akgun</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Katia</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>2019-11-19 10:30:04.306475</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>2020-11-19 10:30:04.306475</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Alroughani</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Raed</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>2019-11-19 10:30:06.035309</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>2020-11-19 10:30:06.035309</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Bass</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Ann</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>2019-11-19 10:30:08.321122</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>2020-11-19 10:30:08.321122</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Berkovich</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Regina</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>2019-11-19 10:30:09.874867</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>2020-11-19 10:30:09.874867</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Broadley</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Simon</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>2019-11-19 10:30:11.627891</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>2020-11-19 10:30:11.627891</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Celius</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Elisabeth</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>2019-11-19 10:30:13.137524</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>2020-11-19 10:30:13.137524</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Temple University</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phladelphia, PA </t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
verfication process if the direcotry exists
</commit_message>
<xml_diff>
--- a/db_check.xlsx
+++ b/db_check.xlsx
@@ -398,10 +398,10 @@
         </is>
       </c>
       <c r="C2" s="2" t="n">
-        <v>43804.43494305822</v>
+        <v>43804.62040354496</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>44170.43494305822</v>
+        <v>44170.62040354496</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -436,10 +436,10 @@
         </is>
       </c>
       <c r="C3" s="2" t="n">
-        <v>43804.43498503239</v>
+        <v>43804.62042361854</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>44170.43498503239</v>
+        <v>44170.62042361854</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -474,10 +474,10 @@
         </is>
       </c>
       <c r="C4" s="2" t="n">
-        <v>43804.4350212731</v>
+        <v>43804.62044560831</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>44170.4350212731</v>
+        <v>44170.62044560831</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -512,10 +512,10 @@
         </is>
       </c>
       <c r="C5" s="2" t="n">
-        <v>43804.43506084823</v>
+        <v>43804.62046317705</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>44170.43506084823</v>
+        <v>44170.62046317705</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -550,10 +550,10 @@
         </is>
       </c>
       <c r="C6" s="2" t="n">
-        <v>43804.43509234616</v>
+        <v>43804.62048405896</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>44170.43509234616</v>
+        <v>44170.62048405896</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -588,10 +588,10 @@
         </is>
       </c>
       <c r="C7" s="2" t="n">
-        <v>43804.43512373529</v>
+        <v>43804.62050764143</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>44170.43512373529</v>
+        <v>44170.62050764143</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -626,10 +626,10 @@
         </is>
       </c>
       <c r="C8" s="2" t="n">
-        <v>43804.4351536918</v>
+        <v>43804.62053384448</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>44170.4351536918</v>
+        <v>44170.62053384448</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -664,10 +664,10 @@
         </is>
       </c>
       <c r="C9" s="2" t="n">
-        <v>43804.43518522081</v>
+        <v>43804.62055432207</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>44170.43518522081</v>
+        <v>44170.62055432207</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -702,10 +702,10 @@
         </is>
       </c>
       <c r="C10" s="2" t="n">
-        <v>43804.43521333184</v>
+        <v>43804.62057781933</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>44170.43521333184</v>
+        <v>44170.62057781933</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -740,10 +740,10 @@
         </is>
       </c>
       <c r="C11" s="2" t="n">
-        <v>43804.43524421235</v>
+        <v>43804.62059922086</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>44170.43524421235</v>
+        <v>44170.62059922086</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -778,10 +778,10 @@
         </is>
       </c>
       <c r="C12" s="2" t="n">
-        <v>43804.43527547179</v>
+        <v>43804.62062163772</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>44170.43527547179</v>
+        <v>44170.62062163772</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -816,10 +816,10 @@
         </is>
       </c>
       <c r="C13" s="2" t="n">
-        <v>43804.43530666122</v>
+        <v>43804.62064129587</v>
       </c>
       <c r="D13" s="2" t="n">
-        <v>44170.43530666122</v>
+        <v>44170.62064129587</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -854,10 +854,10 @@
         </is>
       </c>
       <c r="C14" s="2" t="n">
-        <v>43804.43533704771</v>
+        <v>43804.62067017692</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>44170.43533704771</v>
+        <v>44170.62067017692</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -892,10 +892,10 @@
         </is>
       </c>
       <c r="C15" s="2" t="n">
-        <v>43804.43536957374</v>
+        <v>43804.62068978882</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>44170.43536957374</v>
+        <v>44170.62068978882</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -930,10 +930,10 @@
         </is>
       </c>
       <c r="C16" s="2" t="n">
-        <v>43804.43540154918</v>
+        <v>43804.62071159387</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>44170.43540154918</v>
+        <v>44170.62071159387</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -968,10 +968,10 @@
         </is>
       </c>
       <c r="C17" s="2" t="n">
-        <v>43804.43543137662</v>
+        <v>43804.62073176025</v>
       </c>
       <c r="D17" s="2" t="n">
-        <v>44170.43543137662</v>
+        <v>44170.62073176025</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -1006,10 +1006,10 @@
         </is>
       </c>
       <c r="C18" s="2" t="n">
-        <v>43804.43546021391</v>
+        <v>43804.62076025998</v>
       </c>
       <c r="D18" s="2" t="n">
-        <v>44170.43546021391</v>
+        <v>44170.62076025998</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -1044,10 +1044,10 @@
         </is>
       </c>
       <c r="C19" s="2" t="n">
-        <v>43804.43548980402</v>
+        <v>43804.6207817073</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>44170.43548980402</v>
+        <v>44170.6207817073</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -1082,10 +1082,10 @@
         </is>
       </c>
       <c r="C20" s="2" t="n">
-        <v>43804.43552076308</v>
+        <v>43804.62080901489</v>
       </c>
       <c r="D20" s="2" t="n">
-        <v>44170.43552076308</v>
+        <v>44170.62080901489</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -1120,10 +1120,10 @@
         </is>
       </c>
       <c r="C21" s="2" t="n">
-        <v>43804.43555379265</v>
+        <v>43804.62082906438</v>
       </c>
       <c r="D21" s="2" t="n">
-        <v>44170.43555379265</v>
+        <v>44170.62082906438</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -1219,7 +1219,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:F2"/>
+  <dimension ref="A2:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I9" sqref="I9"/>
@@ -1259,6 +1259,38 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Edwards</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Keith</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>2019-12-05 14:53:53.686462</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2020-12-05 14:53:53.686462</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>MS Center of NE New York</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Latham, NY</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>